<commit_message>
23rd commit - Core alerts - Placeholder and template management TCs
23rd commit - Core alerts - Placeholder and template management TCs
</commit_message>
<xml_diff>
--- a/Testcases/Testcases.xlsx
+++ b/Testcases/Testcases.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\Testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2F9717-5029-4D2F-B1D0-F3EE0472054A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FBAB44-7C68-41FC-B710-7245C59CF030}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{CBD9E713-0ADB-4E71-A875-A1FE3CF6503C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{CBD9E713-0ADB-4E71-A875-A1FE3CF6503C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -34,28 +33,16 @@
     <t>Execute Flag</t>
   </si>
   <si>
-    <t>CollectionAgency.Disposition.CollectionAgencyDisposition_TestClass</t>
-  </si>
-  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>CollectionAgency.AccountAllocation.AgentAccountAllocation_TestClass</t>
-  </si>
-  <si>
-    <t>Core.Configurations.CollectionOfficerConfig_TestClass</t>
   </si>
   <si>
     <t>Test case detailed description</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Core.AlertsandNotifications.AlertsPlaceholderManagement_TestClass</t>
   </si>
   <si>
-    <t>com.test.LoginTest.CoreLoginTest</t>
-  </si>
-  <si>
-    <t>com.test.LoginTest.TestAnyMethod</t>
+    <t>Core.AlertsandNotifications.AlertsTemplateManagement_TestClass</t>
   </si>
 </sst>
 </file>
@@ -499,11 +486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669D0501-9040-441A-85E1-C92B4E260A8C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5A2B89-7AC5-4724-8E7E-CCF989E316F7}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,132 +508,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5A2B89-7AC5-4724-8E7E-CCF989E316F7}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="63.90625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
24th commit - Alerts - Notification management
24th commit - Alerts - Notification management
</commit_message>
<xml_diff>
--- a/Testcases/Testcases.xlsx
+++ b/Testcases/Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\Testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FBAB44-7C68-41FC-B710-7245C59CF030}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01B6506-E175-4472-8DA5-53BF88852F51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{CBD9E713-0ADB-4E71-A875-A1FE3CF6503C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Core.AlertsandNotifications.AlertsTemplateManagement_TestClass</t>
+  </si>
+  <si>
+    <t>Core.AlertsandNotifications.AlertsNotificationManagement_TestClass</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,8 +531,12 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
28th commit - Regression suite update
28th commit - Regression suite update
</commit_message>
<xml_diff>
--- a/Testcases/Testcases.xlsx
+++ b/Testcases/Testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\Testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01B6506-E175-4472-8DA5-53BF88852F51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C18665-75AC-4E5E-B035-73518AA4D105}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{CBD9E713-0ADB-4E71-A875-A1FE3CF6503C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -39,13 +39,16 @@
     <t>Test case detailed description</t>
   </si>
   <si>
-    <t>Core.AlertsandNotifications.AlertsPlaceholderManagement_TestClass</t>
-  </si>
-  <si>
-    <t>Core.AlertsandNotifications.AlertsTemplateManagement_TestClass</t>
-  </si>
-  <si>
-    <t>Core.AlertsandNotifications.AlertsNotificationManagement_TestClass</t>
+    <t>Sl. No</t>
+  </si>
+  <si>
+    <t>Core.AlertsandNotifications.AlertsPlaceholderManagement_TestClass.java</t>
+  </si>
+  <si>
+    <t>Core.AlertsandNotifications.AlertsTemplateManagement_TestClass.java</t>
+  </si>
+  <si>
+    <t>Core.AlertsandNotifications.AlertsNotificationManagement_TestClass.java</t>
   </si>
 </sst>
 </file>
@@ -77,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -117,21 +120,6 @@
       <left style="thick">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
@@ -147,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,10 +158,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -490,97 +477,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5A2B89-7AC5-4724-8E7E-CCF989E316F7}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.90625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.36328125" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.90625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="72.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>